<commit_message>
update com filtro remove cadeiras
</commit_message>
<xml_diff>
--- a/quantidades.xlsx
+++ b/quantidades.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Nome</t>
   </si>
@@ -25,6 +25,12 @@
     <t>Priori</t>
   </si>
   <si>
+    <t>Diferenca</t>
+  </si>
+  <si>
+    <t>porcentagem</t>
+  </si>
+  <si>
     <t>CAFI</t>
   </si>
   <si>
@@ -41,6 +47,39 @@
   </si>
   <si>
     <t>CPLT</t>
+  </si>
+  <si>
+    <t>CABL</t>
+  </si>
+  <si>
+    <t>CCAR</t>
+  </si>
+  <si>
+    <t>CCSA</t>
+  </si>
+  <si>
+    <t>CIGR</t>
+  </si>
+  <si>
+    <t>CIPJ</t>
+  </si>
+  <si>
+    <t>CJBG</t>
+  </si>
+  <si>
+    <t>COLI</t>
+  </si>
+  <si>
+    <t>CPMR</t>
+  </si>
+  <si>
+    <t>CREC</t>
+  </si>
+  <si>
+    <t>CVSA</t>
+  </si>
+  <si>
+    <t>REIF</t>
   </si>
 </sst>
 </file>
@@ -398,13 +437,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,21 +453,33 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>9884</v>
       </c>
       <c r="C2">
-        <v>8353</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>8354</v>
+      </c>
+      <c r="D2">
+        <v>1530</v>
+      </c>
+      <c r="E2">
+        <v>84.52043707001215</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>20476</v>
@@ -436,10 +487,16 @@
       <c r="C3">
         <v>8234</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3">
+        <v>12242</v>
+      </c>
+      <c r="E3">
+        <v>40.21293221332292</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>21167</v>
@@ -447,10 +504,16 @@
       <c r="C4">
         <v>7211</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4">
+        <v>13956</v>
+      </c>
+      <c r="E4">
+        <v>34.06718004440875</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>11963</v>
@@ -458,10 +521,16 @@
       <c r="C5">
         <v>8866</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5">
+        <v>3097</v>
+      </c>
+      <c r="E5">
+        <v>74.11184485496949</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>13878</v>
@@ -469,16 +538,215 @@
       <c r="C6">
         <v>9519</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6">
+        <v>4359</v>
+      </c>
+      <c r="E6">
+        <v>68.59057501080848</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>7212</v>
       </c>
       <c r="C7">
-        <v>4616</v>
+        <v>4620</v>
+      </c>
+      <c r="D7">
+        <v>2592</v>
+      </c>
+      <c r="E7">
+        <v>64.05990016638935</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>3765</v>
+      </c>
+      <c r="C8">
+        <v>2905</v>
+      </c>
+      <c r="D8">
+        <v>860</v>
+      </c>
+      <c r="E8">
+        <v>77.15803452855245</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>12203</v>
+      </c>
+      <c r="C9">
+        <v>4713</v>
+      </c>
+      <c r="D9">
+        <v>7490</v>
+      </c>
+      <c r="E9">
+        <v>38.62165041383266</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>9977</v>
+      </c>
+      <c r="C10">
+        <v>7472</v>
+      </c>
+      <c r="D10">
+        <v>2505</v>
+      </c>
+      <c r="E10">
+        <v>74.89225218001403</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>5045</v>
+      </c>
+      <c r="C11">
+        <v>3374</v>
+      </c>
+      <c r="D11">
+        <v>1671</v>
+      </c>
+      <c r="E11">
+        <v>66.8780971258672</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>15033</v>
+      </c>
+      <c r="C12">
+        <v>8612</v>
+      </c>
+      <c r="D12">
+        <v>6421</v>
+      </c>
+      <c r="E12">
+        <v>57.28730127053815</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>3039</v>
+      </c>
+      <c r="C13">
+        <v>2641</v>
+      </c>
+      <c r="D13">
+        <v>398</v>
+      </c>
+      <c r="E13">
+        <v>86.90358670615333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>3832</v>
+      </c>
+      <c r="C14">
+        <v>2992</v>
+      </c>
+      <c r="D14">
+        <v>840</v>
+      </c>
+      <c r="E14">
+        <v>78.07933194154488</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>3029</v>
+      </c>
+      <c r="C15">
+        <v>1935</v>
+      </c>
+      <c r="D15">
+        <v>1094</v>
+      </c>
+      <c r="E15">
+        <v>63.88246946186861</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>55364</v>
+      </c>
+      <c r="C16">
+        <v>34587</v>
+      </c>
+      <c r="D16">
+        <v>20777</v>
+      </c>
+      <c r="E16">
+        <v>62.47200346795751</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>22583</v>
+      </c>
+      <c r="C17">
+        <v>15069</v>
+      </c>
+      <c r="D17">
+        <v>7514</v>
+      </c>
+      <c r="E17">
+        <v>66.72718416507992</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>19344</v>
+      </c>
+      <c r="C18">
+        <v>7482</v>
+      </c>
+      <c r="D18">
+        <v>11862</v>
+      </c>
+      <c r="E18">
+        <v>38.67866004962779</v>
       </c>
     </row>
   </sheetData>

</xml_diff>